<commit_message>
Built site for kwb.umberto: 0.2.0.9000@254df97
</commit_message>
<xml_diff>
--- a/dev/reference/umberto10_results.xlsx
+++ b/dev/reference/umberto10_results.xlsx
@@ -43,22 +43,22 @@
     <t xml:space="preserve">T07: Centrifuge</t>
   </si>
   <si>
+    <t xml:space="preserve">T14: Polymer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T15: Sludge transport [RER]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T21: fertilizer substitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T31: Electricity credits [ES]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T4: Electricity [IL]</t>
+  </si>
+  <si>
     <t xml:space="preserve">T10: Effluent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T14: Polymer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T15: Sludge transport [RER]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T21: fertilizer substitution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T31: Electricity credits [ES]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T4: Electricity [IL]</t>
   </si>
   <si>
     <t xml:space="preserve">ReCiPe Midpoint (H) w/o LT - freshwater ecotoxicity w/o LT, FETPinf w/o LT</t>
@@ -465,7 +465,9 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" t="n">
+        <v>392609.350571056</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -475,7 +477,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>392609.350571056</v>
+        <v>110.077708792406</v>
       </c>
     </row>
     <row r="7">
@@ -486,7 +488,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>110.077708792406</v>
+        <v>-217231.523240712</v>
       </c>
     </row>
     <row r="8">
@@ -497,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>-217231.523240712</v>
+        <v>-1172632.84519849</v>
       </c>
     </row>
     <row r="9">
@@ -508,7 +510,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-1172632.84519849</v>
+        <v>13314949.1388226</v>
       </c>
     </row>
     <row r="10">
@@ -518,9 +520,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>13314949.1388226</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -552,46 +552,54 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>281.204698933857</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3"/>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0843318098494594</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-2759.6585950617</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-308.271724439994</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>281.204698933857</v>
+        <v>2056.05362640351</v>
       </c>
     </row>
     <row r="7">
@@ -599,33 +607,27 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.0843318098494594</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-2759.6585950617</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-308.271724439994</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -634,9 +636,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>2056.05362640351</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -668,37 +668,43 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
+        <v>12</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3009.67715207925</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3"/>
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8.99061191069666</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.00160311891525617</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>3009.67715207925</v>
+        <v>1860.96549371055</v>
       </c>
     </row>
     <row r="6">
@@ -706,10 +712,10 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>8.99061191069666</v>
+        <v>-54.0808142552251</v>
       </c>
     </row>
     <row r="7">
@@ -717,10 +723,10 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00160311891525617</v>
+        <v>770.450190589926</v>
       </c>
     </row>
     <row r="8">
@@ -728,33 +734,27 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1860.96549371055</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-54.0808142552251</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="n">
-        <v>770.450190589926</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -786,46 +786,54 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>23784.5824592949</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3"/>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>23.22929811789</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-110027.964095341</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-75226.2696774404</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>23784.5824592949</v>
+        <v>571686.709419825</v>
       </c>
     </row>
     <row r="7">
@@ -833,33 +841,27 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>23.22929811789</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-110027.964095341</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-75226.2696774404</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -868,9 +870,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>571686.709419825</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -902,46 +902,54 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>384.798405223609</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3"/>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.391233296339834</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-1821.71691243872</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-548.779480037789</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>384.798405223609</v>
+        <v>3172.68059006507</v>
       </c>
     </row>
     <row r="7">
@@ -949,33 +957,27 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.391233296339834</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-1821.71691243872</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-548.779480037789</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -984,9 +986,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>3172.68059006507</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1040,9 +1040,11 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>12</v>
+      </c>
+      <c r="C4" t="n">
+        <v>261651.314309439</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -1052,7 +1054,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>261651.314309439</v>
+        <v>1437.33152509733</v>
       </c>
     </row>
     <row r="6">
@@ -1063,7 +1065,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>1437.33152509733</v>
+        <v>0.0139564028473857</v>
       </c>
     </row>
     <row r="7">
@@ -1074,7 +1076,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0139564028473857</v>
+        <v>10612.5042510072</v>
       </c>
     </row>
     <row r="8">
@@ -1085,7 +1087,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>10612.5042510072</v>
+        <v>-171.380370107561</v>
       </c>
     </row>
     <row r="9">
@@ -1096,7 +1098,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>-171.380370107561</v>
+        <v>1393.38228094482</v>
       </c>
     </row>
     <row r="10">
@@ -1104,11 +1106,9 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1393.38228094482</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1162,28 +1162,32 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2142.13681635859</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5"/>
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.34340773994572</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>2142.13681635859</v>
+        <v>33056.0200547611</v>
       </c>
     </row>
     <row r="7">
@@ -1191,10 +1195,10 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>0.34340773994572</v>
+        <v>-8259.3853040454</v>
       </c>
     </row>
     <row r="8">
@@ -1202,10 +1206,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>33056.0200547611</v>
+        <v>74116.3582598173</v>
       </c>
     </row>
     <row r="9">
@@ -1213,11 +1217,9 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-8259.3853040454</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -1226,9 +1228,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>74116.3582598173</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1260,46 +1260,54 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>10433116.9438371</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3"/>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1762.82923822559</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-7072323.08092806</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-13154124.1204715</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>10433116.9438371</v>
+        <v>181431756.306697</v>
       </c>
     </row>
     <row r="7">
@@ -1307,33 +1315,27 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1762.82923822559</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-7072323.08092806</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-13154124.1204715</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -1342,9 +1344,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>181431756.306697</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1376,46 +1376,54 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>296075.355505227</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3"/>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>38.8605254313039</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4"/>
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-712713.211781755</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-12325698.9368461</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>296075.355505227</v>
+        <v>542344.893745249</v>
       </c>
     </row>
     <row r="7">
@@ -1423,33 +1431,27 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="n">
-        <v>38.8605254313039</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="n">
-        <v>-712713.211781755</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C8"/>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-12325698.9368461</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -1458,9 +1460,7 @@
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="n">
-        <v>542344.893745249</v>
-      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>